<commit_message>
refactor : fix typo
</commit_message>
<xml_diff>
--- a/public/template_supplier.xlsx
+++ b/public/template_supplier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46FDE30-55B7-4E2D-B2E7-F0175ADB1F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4663ED-57B7-4E9B-94B1-B6EF88C0001A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,14 +350,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -404,14 +404,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
+    <row r="5" spans="1:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>